<commit_message>
Update list of parts
</commit_message>
<xml_diff>
--- a/KiCad_and_production_files/MicroZed_carrier_board_v4_parts.xlsx
+++ b/KiCad_and_production_files/MicroZed_carrier_board_v4_parts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vniko\Google Drive\Work\Arduino\KiCad files\MicroZed_carrier_board\MicroZed_carrier_board_v4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6494728-1109-47D8-A57D-F2DDCE7CB4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16A41BE-BA74-4DCA-86F4-8C6D6A8D004E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="340" windowWidth="34540" windowHeight="20460" xr2:uid="{3D863549-0935-41B1-B88A-2C86AFE9A734}"/>
+    <workbookView xWindow="2660" yWindow="1140" windowWidth="34540" windowHeight="20460" xr2:uid="{3D863549-0935-41B1-B88A-2C86AFE9A734}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -644,9 +644,6 @@
     <t>power indicators, RX_to_FPGA</t>
   </si>
   <si>
-    <t>Following connectors are not part of BOM, i.e. not part of JLCPCB Assembly (they are intended for DYI hand soldering):</t>
-  </si>
-  <si>
     <t>SSW-119-01-F-D</t>
   </si>
   <si>
@@ -654,6 +651,9 @@
   </si>
   <si>
     <t>JP1</t>
+  </si>
+  <si>
+    <t>Following connectors are not part of BOM, i.e. not part of JLCPCB Assembly (they are intended for DIY hand soldering):</t>
   </si>
 </sst>
 </file>
@@ -747,7 +747,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -800,16 +800,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1923,22 +1917,15 @@
       <c r="F45" s="12"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A46" s="18"/>
-      <c r="B46" s="18"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="20"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="18"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="18"/>
     </row>
     <row r="47" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A47" s="21" t="s">
-        <v>202</v>
-      </c>
-      <c r="B47" s="18"/>
-      <c r="C47" s="19"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
+      <c r="A47" s="19" t="s">
+        <v>205</v>
+      </c>
+      <c r="C47" s="4"/>
+      <c r="D47" s="18"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C48" s="4"/>
@@ -1967,7 +1954,7 @@
       <c r="C50" s="11"/>
       <c r="D50" s="10"/>
       <c r="E50" s="10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
@@ -1980,7 +1967,7 @@
       <c r="C51" s="11"/>
       <c r="D51" s="10"/>
       <c r="E51" s="10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
@@ -1988,7 +1975,7 @@
         <v>73</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C52" s="11"/>
       <c r="D52" s="10"/>

</xml_diff>